<commit_message>
html and php of pinyin is done
</commit_message>
<xml_diff>
--- a/public/Excel/excel.xlsx
+++ b/public/Excel/excel.xlsx
@@ -3,24 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCAD6D1-CC55-44C3-82B7-699F7620C736}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFABB4B7-C006-4C0C-BE38-62317C0E15CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="347">
   <si>
     <t>李嘉宁</t>
   </si>
@@ -539,13 +544,708 @@
   </si>
   <si>
     <t>朱子叶</t>
+  </si>
+  <si>
+    <t>Li Jianing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Yiyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lie La</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Song Zigui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tao Anzhe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Hanqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Jiayi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yao Mengxi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Yueqian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Song Qi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Su Annan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Aoxuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xinran</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yan Shuo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Guang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Jingqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Kuo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Tianyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhong Zelin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Cao Rui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fei Aiwen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hao Xinyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Huang Yixin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jin Yiming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma Xinyao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wan Siqing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Xiaoyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Du Yuxuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duo Yongxing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guo Jingyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He Cheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He Runyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Chengcheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luan Jieming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Haoxuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qi Xu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhao Yuxiong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dou Kaiwen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hao Deming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chen Siheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guan Weiheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qu Yuezhou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Hao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yin Sihong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chang Jingqian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Du Zhiyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiang Qiange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Jiayin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Jiayue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xie Yuqing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu Ziyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Yimei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wen Ping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qiu Zihe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Siyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Yingjia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dong Keyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geng Zibo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Chenghao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Jinghan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yihao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qiang Jingyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei Zichen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Jingyun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu Wenjing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chen Hanyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gao Chi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hao Guanghua</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He Mingrui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Zhenzhuo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma Siqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Niu Tianxiao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xiaoyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Yaxuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Chuhan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu Ruiqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Kaiqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Haozhe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Zhuoqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhou Jingyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhou Shuyao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhou Yufei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cao Yuxin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jia Peining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Naye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Sijia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Tongxin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Yanlin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Yuchen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He Ruilin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shen Jingqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sun Yutong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Chuwen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xinyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Zehao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Jiangxue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xinou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Yudan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xie Tianyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu Shixin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ye Xingchen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bi Chenming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gao Xiaodong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiang Yuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yifan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Su Yukun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tang Mohan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Dongjun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Zheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yao Ruoqing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yu Xinhang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Xueyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhao Zejun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zheng Jie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xingze</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dong Zhilin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Hongyue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yuting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma Shiyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Jingwen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Yanruo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Yuheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhao Wanjun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zou Yaxin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cao Xinyuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cao Jiaxi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liang Zhongyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Chengkun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Qingyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qi Shilong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Su Yige</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhao Ziqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu Haodong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheng Kaiyuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chen Yixuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deng Zixuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dong Hantong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gao Yang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guo Tianyue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guo Xiao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meng Zongye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Zhiyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Ziyun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Hanxiao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Xilin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Zhuoyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ye Ming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Ruihan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Zihan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Ziyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Zheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fang Shen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Huang Yuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Liman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sun Xiaomeng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Zishi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yu Ke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhang Yanyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhou Runwei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ge Hongyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Yuelin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luo Dan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mi Jingyao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shen Yihui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei Zixiong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fan Wenkai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Tunan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peng Jiaqi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wang Xuening</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu Yiyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Yuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhu Zhiyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhu Ziye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,6 +1270,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -618,22 +1326,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -916,905 +1624,1974 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A182"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="5">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" s="5">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="5">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="5">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" s="5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C38" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C44" s="5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C45" s="5">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C48" s="5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C50" s="5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C51" s="5">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C52" s="5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C53" s="5">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C54" s="5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+      <c r="B56" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" s="5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C58" s="5">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C59" s="5">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" s="5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C61" s="5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C62" s="5">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="B63" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C63" s="5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C64" s="5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="5">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="B67" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C67" s="5">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="6"/>
+      <c r="B68" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="B69" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C69" s="5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+      <c r="B70" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C70" s="5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+      <c r="B71" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C71" s="5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+      <c r="B72" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C72" s="5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="B73" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C73" s="5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="B74" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" s="5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+      <c r="B75" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C75" s="5">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+      <c r="B76" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C76" s="5">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+      <c r="B77" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+      <c r="B78" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C78" s="5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+      <c r="B79" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C79" s="5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+      <c r="B80" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C80" s="5">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+      <c r="B81" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C81" s="5">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+      <c r="B82" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C82" s="5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+      <c r="B83" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" s="5">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="B84" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" s="5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
+      <c r="B85" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
+      <c r="B86" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C86" s="5">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="B88" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C88" s="5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+      <c r="B89" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C89" s="5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+      <c r="B90" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C90" s="5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
+      <c r="B91" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C91" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="B92" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="6" t="s">
+      <c r="B93" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="5">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="6" t="s">
+      <c r="B94" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C94" s="5">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="6" t="s">
+      <c r="B95" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C95" s="5">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="6" t="s">
+      <c r="B96" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C96" s="5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="6" t="s">
+      <c r="B97" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C97" s="5">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="6" t="s">
+      <c r="B98" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C98" s="5">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="6" t="s">
+      <c r="B99" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" s="5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="6" t="s">
+      <c r="B100" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C100" s="5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+      <c r="B101" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C101" s="5">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="6" t="s">
+      <c r="B102" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C102" s="5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="6" t="s">
+      <c r="B103" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C103" s="5">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+      <c r="B104" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C104" s="5">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="6" t="s">
+      <c r="B105" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C105" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="2"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B106" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C106" s="5">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="6"/>
+      <c r="B107" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B108" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C108" s="5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B109" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C109" s="5">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C110" s="5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B111" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C111" s="5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B112" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C112" s="5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B113" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C113" s="5">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B114" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C114" s="5">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B115" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" s="5">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B116" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C116" s="5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B117" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C117" s="5">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B118" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C118" s="5">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B119" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C119" s="5">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B120" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C120" s="5">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B121" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C121" s="5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="6"/>
+      <c r="B122" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B123" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C123" s="5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B124" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C124" s="5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B125" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C125" s="5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B126" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C126" s="5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B127" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C127" s="5">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C128" s="5">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C129" s="5">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C130" s="5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C131" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B132" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C132" s="5">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B133" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C133" s="5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B134" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C134" s="5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B135" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C135" s="5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B136" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C136" s="5">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B137" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C137" s="5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B138" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C138" s="5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B139" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C139" s="5">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B140" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C140" s="5">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="2"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B141" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C141" s="5">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="6"/>
+      <c r="B142" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B143" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C143" s="5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B144" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C144" s="5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B145" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C145" s="5">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C146" s="5">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C147" s="5">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C148" s="5">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C149" s="5">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C150" s="5">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C151" s="5">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C152" s="5">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C153" s="5">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C154" s="5">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C155" s="5">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C156" s="5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C157" s="5">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C158" s="5">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C159" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C160" s="5">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C161" s="5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C162" s="5">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C163" s="5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C164" s="5">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C165" s="5">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C166" s="5">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="2"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C167" s="5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="6"/>
+      <c r="B168" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C169" s="5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C170" s="5">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C171" s="5">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C172" s="5">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C173" s="5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C174" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C175" s="5">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C176" s="5">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C177" s="5">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C178" s="5">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C179" s="5">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C180" s="5">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C181" s="5">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>172</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C182" s="5">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>